<commit_message>
Overhual of the debug system. More reporting fixes. Started new PLC module setup for creating the IO tree.
</commit_message>
<xml_diff>
--- a/CnE2PLC.Reporting/CnE_Template.xlsx
+++ b/CnE2PLC.Reporting/CnE_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwp00\source\repos\CnE2PLC_master\CnE2PLC.Reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NONGME\source\repos\CnE2PLC\CnE2PLC.Reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ABCDDE-943A-40FA-947D-FCA7AEA3C3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50F4BA4-4C85-4CD2-BC96-9A1AA003CE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="236" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="236" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank Battery" sheetId="32" r:id="rId1"/>
@@ -35,13 +35,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Govindarajulu, Madhan (Abu Dhabi) - Personal View" guid="{84BD1099-CF0B-4C23-9CBE-24383677C50A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="739" tabRatio="506" activeSheetId="6"/>
+    <customWorkbookView name="Patel, Jetul (Abu Dhabi) - Personal View" guid="{79E8904F-E8B8-4A6D-BD16-944ADFDD4480}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="799" tabRatio="506" activeSheetId="6"/>
+    <customWorkbookView name="Bhatt, Nimesh (Abu Dhabi) - Personal View" guid="{97D85B01-99B0-4FB9-AF85-0571ADEF4646}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="815" tabRatio="506" activeSheetId="6"/>
+    <customWorkbookView name="Shah, Harshit (Abu Dhabi) - Personal View" guid="{61854588-8877-42CD-B97D-5251954528B8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1218" windowHeight="718" tabRatio="506" activeSheetId="6"/>
+    <customWorkbookView name="Dandala, Sonu (Abu Dhabi) - Personal View" guid="{B0AC76D0-1760-47B4-8B47-41ADE471937C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" tabRatio="506" activeSheetId="6"/>
+    <customWorkbookView name="Pillarisetti, Parthasaradhi (Abu Dhabi) - Personal View" guid="{B0724FAF-C1FC-4D80-9449-B556164F4BBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="799" tabRatio="506" activeSheetId="6"/>
     <customWorkbookView name="Talekar, Mangesh (Abu Dhabi) - Personal View" guid="{B1B8974D-5FB1-4624-BA06-EE0547942650}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="815" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Pillarisetti, Parthasaradhi (Abu Dhabi) - Personal View" guid="{B0724FAF-C1FC-4D80-9449-B556164F4BBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="799" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Dandala, Sonu (Abu Dhabi) - Personal View" guid="{B0AC76D0-1760-47B4-8B47-41ADE471937C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Shah, Harshit (Abu Dhabi) - Personal View" guid="{61854588-8877-42CD-B97D-5251954528B8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1218" windowHeight="718" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Bhatt, Nimesh (Abu Dhabi) - Personal View" guid="{97D85B01-99B0-4FB9-AF85-0571ADEF4646}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="815" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Patel, Jetul (Abu Dhabi) - Personal View" guid="{79E8904F-E8B8-4A6D-BD16-944ADFDD4480}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="799" tabRatio="506" activeSheetId="6"/>
-    <customWorkbookView name="Govindarajulu, Madhan (Abu Dhabi) - Personal View" guid="{84BD1099-CF0B-4C23-9CBE-24383677C50A}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="739" tabRatio="506" activeSheetId="6"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1145,6 +1145,99 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1154,9 +1247,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1164,9 +1254,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,99 +1261,22 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1302,13 +1312,15 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <strike/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1625,7 +1637,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="11.25"/>
@@ -1655,27 +1667,27 @@
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="48"/>
       <c r="Q1" s="39"/>
       <c r="R1" s="40"/>
     </row>
@@ -1692,37 +1704,37 @@
       <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="80" t="s">
+      <c r="M2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="58" t="s">
+      <c r="O2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="60" t="s">
+      <c r="P2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="51" t="s">
+      <c r="Q2" s="80" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="41"/>
@@ -1740,19 +1752,19 @@
       <c r="D3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="52"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="81"/>
       <c r="R3" s="42"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -1768,23 +1780,23 @@
       <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="52"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="63"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="81"/>
       <c r="R4" s="42"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -1800,23 +1812,23 @@
       <c r="D5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="52"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="63"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="81"/>
       <c r="R5" s="42"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1">
@@ -1832,29 +1844,29 @@
       <c r="D6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="52"/>
+      <c r="E6" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="61"/>
+      <c r="I6" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="63"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="81"/>
       <c r="R6" s="42"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A7" s="43"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
@@ -1864,29 +1876,29 @@
       <c r="D7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="54"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="52"/>
+      <c r="E7" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="63"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="81"/>
       <c r="R7" s="42"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
-      <c r="A8" s="44"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="12" t="s">
         <v>28</v>
       </c>
@@ -1896,29 +1908,29 @@
       <c r="D8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="52"/>
+      <c r="E8" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="63"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="81"/>
       <c r="R8" s="42"/>
     </row>
     <row r="9" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A9" s="44"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
@@ -1928,29 +1940,29 @@
       <c r="D9" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="46"/>
-      <c r="I9" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="52"/>
+      <c r="E9" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="63"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="81"/>
       <c r="R9" s="42"/>
     </row>
     <row r="10" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="44"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
@@ -1960,29 +1972,29 @@
       <c r="D10" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="52"/>
+      <c r="E10" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="63"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="81"/>
       <c r="R10" s="42"/>
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
-      <c r="A11" s="44"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
@@ -1992,29 +2004,29 @@
       <c r="D11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="52"/>
+      <c r="E11" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="63"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="81"/>
       <c r="R11" s="42"/>
     </row>
     <row r="12" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="45"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="13" t="s">
         <v>32</v>
       </c>
@@ -2022,84 +2034,84 @@
         <v>99</v>
       </c>
       <c r="D12" s="20"/>
-      <c r="E12" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="52"/>
+      <c r="E12" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="81"/>
       <c r="R12" s="42"/>
     </row>
     <row r="13" spans="1:18" s="1" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="62" t="s">
+      <c r="H13" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="62" t="s">
+      <c r="J13" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="64" t="s">
+      <c r="K13" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="78"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="60"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="66"/>
       <c r="Q13" s="33" t="s">
         <v>43</v>
       </c>
       <c r="R13" s="30"/>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="61"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="67"/>
       <c r="Q14" s="35" t="s">
         <v>44</v>
       </c>
@@ -2149,6 +2161,44 @@
   <autoFilter ref="A14:R15" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <dataConsolidate/>
   <mergeCells count="54">
+    <mergeCell ref="Q2:Q12"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="P2:P14"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="E12:F12"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="E2:F2"/>
@@ -2165,68 +2215,15 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="O2:O14"/>
-    <mergeCell ref="P2:P14"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="Q2:Q12"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:E16 G16:O16 R16">
-    <cfRule type="expression" dxfId="5" priority="8">
-      <formula>$F16="Under Review"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
-      <formula>$F16="Approved Deviation"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="10">
-      <formula>$F16="Standard IO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
-      <formula>$F16="New Project"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>$F16="Not In Use"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R14:R16 R2:R12">
-    <cfRule type="expression" dxfId="1" priority="6">
+  <conditionalFormatting sqref="R2:R12 R14:R16">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>R$13="NO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
-      <formula>R$13="NEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -2243,21 +2240,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AE668B9594F484BBC3A2C1658CF2A9E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67ab95564bb708393136f54ac7b7f428">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92abb93a-84ef-4449-994b-44d11a02ca42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e0b3638fb6e1b7a7114254ab1408a7f" ns2:_="">
     <xsd:import namespace="92abb93a-84ef-4449-994b-44d11a02ca42"/>
@@ -2397,10 +2379,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8991FB34-536E-4327-8CBB-E8DFE1E7BA20}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0FE22CA-7BAA-4575-869B-91E7FB37BDEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92abb93a-84ef-4449-994b-44d11a02ca42"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2422,19 +2429,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0FE22CA-7BAA-4575-869B-91E7FB37BDEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8991FB34-536E-4327-8CBB-E8DFE1E7BA20}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="92abb93a-84ef-4449-994b-44d11a02ca42"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>